<commit_message>
Add potential depots count
</commit_message>
<xml_diff>
--- a/data/demo2/Data info(1).xlsx
+++ b/data/demo2/Data info(1).xlsx
@@ -288,10 +288,10 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="5">
     <numFmt numFmtId="176" formatCode="0.000"/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="178" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="178" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="23">
     <font>
@@ -323,19 +323,26 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="3"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -346,16 +353,16 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
       <name val="Calibri"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
       <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -370,7 +377,52 @@
     </font>
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -392,68 +444,16 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
       <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -482,49 +482,127 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -536,31 +614,37 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -572,97 +656,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -685,11 +685,26 @@
       <diagonal/>
     </border>
     <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
       <top/>
-      <bottom style="medium">
-        <color theme="4"/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -705,6 +720,30 @@
       </top>
       <bottom style="thin">
         <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -735,45 +774,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top/>
@@ -785,148 +785,148 @@
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="14" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="5" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="9" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="10" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1747,7 +1747,7 @@
     <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
       <pane xSplit="1" topLeftCell="C1" activePane="topRight" state="frozen"/>
       <selection/>
-      <selection pane="topRight" activeCell="K33" sqref="K33"/>
+      <selection pane="topRight" activeCell="M34" sqref="M34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14"/>
@@ -2665,7 +2665,7 @@
         <v>11125.402</v>
       </c>
     </row>
-    <row r="33" spans="1:9">
+    <row r="33" spans="1:11">
       <c r="A33" t="s">
         <v>58</v>
       </c>
@@ -2690,8 +2690,14 @@
       <c r="I33" s="9">
         <v>1725.609</v>
       </c>
-    </row>
-    <row r="34" spans="1:9">
+      <c r="J33">
+        <v>4877.86</v>
+      </c>
+      <c r="K33">
+        <v>4869.873</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11">
       <c r="A34" t="s">
         <v>59</v>
       </c>
@@ -2716,8 +2722,14 @@
       <c r="I34" s="9">
         <v>4026.539</v>
       </c>
-    </row>
-    <row r="35" spans="1:9">
+      <c r="J34">
+        <v>7141.88</v>
+      </c>
+      <c r="K34">
+        <v>7183.734</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11">
       <c r="A35" t="s">
         <v>60</v>
       </c>
@@ -2742,8 +2754,14 @@
       <c r="I35" s="9">
         <v>5970.177</v>
       </c>
-    </row>
-    <row r="36" spans="1:9">
+      <c r="J35">
+        <v>9235.29</v>
+      </c>
+      <c r="K35">
+        <v>9588.401</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11">
       <c r="A36" t="s">
         <v>61</v>
       </c>
@@ -2767,6 +2785,12 @@
       </c>
       <c r="I36" s="9">
         <v>9375.874</v>
+      </c>
+      <c r="J36">
+        <v>11643.69</v>
+      </c>
+      <c r="K36">
+        <v>11406.992</v>
       </c>
     </row>
   </sheetData>

</xml_diff>